<commit_message>
Added USA Swimming and PNS logos, and made some adjustments to the header layout for better mobile display. Also updated the Excel file with new situations and resolutions.
</commit_message>
<xml_diff>
--- a/Situations-n-Resolutions-with-sections.xlsx
+++ b/Situations-n-Resolutions-with-sections.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="375">
   <si>
-    <t xml:space="preserve">Section</t>
+    <t xml:space="preserve">Stroke</t>
   </si>
   <si>
     <t xml:space="preserve">Number</t>
@@ -1171,6 +1171,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1192,6 +1193,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1236,16 +1238,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1379,2551 +1385,2551 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A71" activeCellId="0" sqref="A71"/>
-      <selection pane="bottomRight" activeCell="D45" activeCellId="0" sqref="D45"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="64.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="67.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="122.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="64.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="67.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="122.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.55"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="13" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="E22" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="E23" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="0" t="n">
+      <c r="B24" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="0" t="s">
+      <c r="E24" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="B25" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E25" s="0" t="s">
+      <c r="E25" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="E26" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="E27" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="0" t="n">
+      <c r="B28" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="E28" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="0" t="n">
+      <c r="B29" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E29" s="0" t="s">
+      <c r="E29" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="0" t="n">
+      <c r="B30" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E30" s="0" t="s">
+      <c r="E30" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="0" t="n">
+      <c r="B31" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="0" t="s">
+      <c r="D31" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E31" s="0" t="s">
+      <c r="E31" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="0" t="n">
+      <c r="B32" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D32" s="0" t="s">
+      <c r="D32" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E32" s="0" t="s">
+      <c r="E32" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="0" t="n">
+      <c r="B33" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D33" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E33" s="0" t="s">
+      <c r="E33" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="0" t="n">
+      <c r="B34" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C34" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="D34" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E34" s="0" t="s">
+      <c r="E34" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="0" t="n">
+      <c r="B35" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D35" s="0" t="s">
+      <c r="D35" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E35" s="0" t="s">
+      <c r="E35" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="0" t="n">
+      <c r="B36" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D36" s="0" t="s">
+      <c r="D36" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E36" s="0" t="s">
+      <c r="E36" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="0" t="n">
+      <c r="B37" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D37" s="0" t="s">
+      <c r="D37" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E37" s="0" t="s">
+      <c r="E37" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B38" s="0" t="n">
+      <c r="B38" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D38" s="0" t="s">
+      <c r="D38" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E38" s="0" t="s">
+      <c r="E38" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B39" s="0" t="n">
+      <c r="B39" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D39" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E39" s="0" t="s">
+      <c r="E39" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B40" s="0" t="n">
+      <c r="B40" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="C40" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="D40" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E40" s="0" t="s">
+      <c r="E40" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B41" s="0" t="n">
+      <c r="B41" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C41" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D41" s="0" t="s">
+      <c r="D41" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E41" s="0" t="s">
+      <c r="E41" s="1" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B42" s="0" t="n">
+      <c r="B42" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="C42" s="0" t="s">
+      <c r="C42" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D42" s="0" t="s">
+      <c r="D42" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E42" s="0" t="s">
+      <c r="E42" s="1" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B43" s="0" t="n">
+      <c r="B43" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C43" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D43" s="0" t="s">
+      <c r="D43" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E43" s="0" t="s">
+      <c r="E43" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B44" s="0" t="n">
+      <c r="B44" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C44" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D44" s="0" t="s">
+      <c r="D44" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E44" s="0" t="s">
+      <c r="E44" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+    <row r="45" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B45" s="0" t="n">
+      <c r="B45" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="D45" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E45" s="0" t="s">
+      <c r="E45" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B46" s="0" t="n">
+      <c r="B46" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D46" s="0" t="s">
+      <c r="D46" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E46" s="0" t="s">
+      <c r="E46" s="1" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B47" s="0" t="n">
+      <c r="B47" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D47" s="0" t="s">
+      <c r="D47" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E47" s="0" t="s">
+      <c r="E47" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B48" s="0" t="n">
+      <c r="B48" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="C48" s="0" t="s">
+      <c r="C48" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D48" s="0" t="s">
+      <c r="D48" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E48" s="0" t="s">
+      <c r="E48" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B49" s="0" t="n">
+      <c r="B49" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="C49" s="0" t="s">
+      <c r="C49" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D49" s="0" t="s">
+      <c r="D49" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="E49" s="0" t="s">
+      <c r="E49" s="1" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B50" s="0" t="n">
+      <c r="B50" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="C50" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D50" s="0" t="s">
+      <c r="D50" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E50" s="0" t="s">
+      <c r="E50" s="1" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B51" s="0" t="n">
+      <c r="B51" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="C51" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D51" s="0" t="s">
+      <c r="D51" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E51" s="0" t="s">
+      <c r="E51" s="1" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B52" s="0" t="n">
+      <c r="B52" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="C52" s="0" t="s">
+      <c r="C52" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D52" s="0" t="s">
+      <c r="D52" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E52" s="0" t="s">
+      <c r="E52" s="1" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B53" s="0" t="n">
+      <c r="B53" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="C53" s="0" t="s">
+      <c r="C53" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D53" s="0" t="s">
+      <c r="D53" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E53" s="0" t="s">
+      <c r="E53" s="1" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B54" s="0" t="n">
+      <c r="B54" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="C54" s="0" t="s">
+      <c r="C54" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D54" s="0" t="s">
+      <c r="D54" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E54" s="0" t="s">
+      <c r="E54" s="1" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="A55" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B55" s="0" t="n">
+      <c r="B55" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="C55" s="0" t="s">
+      <c r="C55" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="D55" s="0" t="s">
+      <c r="D55" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E55" s="0" t="s">
+      <c r="E55" s="1" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B56" s="0" t="n">
+      <c r="B56" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="C56" s="0" t="s">
+      <c r="C56" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D56" s="0" t="s">
+      <c r="D56" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E56" s="0" t="s">
+      <c r="E56" s="1" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="A57" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B57" s="0" t="n">
+      <c r="B57" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="C57" s="0" t="s">
+      <c r="C57" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D57" s="0" t="s">
+      <c r="D57" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E57" s="0" t="s">
+      <c r="E57" s="1" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+      <c r="A58" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B58" s="0" t="n">
+      <c r="B58" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="C58" s="0" t="s">
+      <c r="C58" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D58" s="0" t="s">
+      <c r="D58" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E58" s="0" t="s">
+      <c r="E58" s="1" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+      <c r="A59" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B59" s="0" t="n">
+      <c r="B59" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="C59" s="0" t="s">
+      <c r="C59" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D59" s="0" t="s">
+      <c r="D59" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E59" s="0" t="s">
+      <c r="E59" s="1" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+      <c r="A60" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B60" s="0" t="n">
+      <c r="B60" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="C60" s="0" t="s">
+      <c r="C60" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D60" s="0" t="s">
+      <c r="D60" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E60" s="0" t="s">
+      <c r="E60" s="1" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+      <c r="A61" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B61" s="0" t="n">
+      <c r="B61" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="C61" s="0" t="s">
+      <c r="C61" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D61" s="0" t="s">
+      <c r="D61" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E61" s="0" t="s">
+      <c r="E61" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+      <c r="A62" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B62" s="0" t="n">
+      <c r="B62" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="C62" s="0" t="s">
+      <c r="C62" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D62" s="0" t="s">
+      <c r="D62" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E62" s="0" t="s">
+      <c r="E62" s="1" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="A63" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B63" s="0" t="n">
+      <c r="B63" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="C63" s="0" t="s">
+      <c r="C63" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D63" s="0" t="s">
+      <c r="D63" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E63" s="0" t="s">
+      <c r="E63" s="1" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="A64" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B64" s="0" t="n">
+      <c r="B64" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="C64" s="0" t="s">
+      <c r="C64" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D64" s="0" t="s">
+      <c r="D64" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E64" s="0" t="s">
+      <c r="E64" s="1" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+      <c r="A65" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B65" s="0" t="n">
+      <c r="B65" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="C65" s="0" t="s">
+      <c r="C65" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="D65" s="0" t="s">
+      <c r="D65" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E65" s="0" t="s">
+      <c r="E65" s="1" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+      <c r="A66" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B66" s="0" t="n">
+      <c r="B66" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="C66" s="0" t="s">
+      <c r="C66" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D66" s="0" t="s">
+      <c r="D66" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="E66" s="0" t="s">
+      <c r="E66" s="1" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+      <c r="A67" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B67" s="0" t="n">
+      <c r="B67" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="C67" s="0" t="s">
+      <c r="C67" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="D67" s="0" t="s">
+      <c r="D67" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E67" s="0" t="s">
+      <c r="E67" s="1" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+      <c r="A68" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B68" s="0" t="n">
+      <c r="B68" s="1" t="n">
         <v>67</v>
       </c>
-      <c r="C68" s="0" t="s">
+      <c r="C68" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D68" s="0" t="s">
+      <c r="D68" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E68" s="0" t="s">
+      <c r="E68" s="1" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+      <c r="A69" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B69" s="0" t="n">
+      <c r="B69" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="C69" s="0" t="s">
+      <c r="C69" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="D69" s="0" t="s">
+      <c r="D69" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E69" s="0" t="s">
+      <c r="E69" s="1" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+      <c r="A70" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B70" s="0" t="n">
+      <c r="B70" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="C70" s="0" t="s">
+      <c r="C70" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="D70" s="0" t="s">
+      <c r="D70" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E70" s="0" t="s">
+      <c r="E70" s="1" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+      <c r="A71" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B71" s="0" t="n">
+      <c r="B71" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="C71" s="0" t="s">
+      <c r="C71" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="D71" s="0" t="s">
+      <c r="D71" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="E71" s="0" t="s">
+      <c r="E71" s="1" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+      <c r="A72" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B72" s="0" t="n">
+      <c r="B72" s="1" t="n">
         <v>71</v>
       </c>
-      <c r="C72" s="0" t="s">
+      <c r="C72" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="D72" s="0" t="s">
+      <c r="D72" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E72" s="0" t="s">
+      <c r="E72" s="1" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+      <c r="A73" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B73" s="0" t="n">
+      <c r="B73" s="1" t="n">
         <v>72</v>
       </c>
-      <c r="C73" s="0" t="s">
+      <c r="C73" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="D73" s="0" t="s">
+      <c r="D73" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E73" s="0" t="s">
+      <c r="E73" s="1" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+      <c r="A74" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B74" s="0" t="n">
+      <c r="B74" s="1" t="n">
         <v>73</v>
       </c>
-      <c r="C74" s="0" t="s">
+      <c r="C74" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="D74" s="0" t="s">
+      <c r="D74" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E74" s="0" t="s">
+      <c r="E74" s="1" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+      <c r="A75" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B75" s="0" t="n">
+      <c r="B75" s="1" t="n">
         <v>74</v>
       </c>
-      <c r="C75" s="0" t="s">
+      <c r="C75" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="D75" s="0" t="s">
+      <c r="D75" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="E75" s="0" t="s">
+      <c r="E75" s="1" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+      <c r="A76" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B76" s="0" t="n">
+      <c r="B76" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="C76" s="0" t="s">
+      <c r="C76" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D76" s="0" t="s">
+      <c r="D76" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E76" s="0" t="s">
+      <c r="E76" s="1" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+      <c r="A77" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B77" s="0" t="n">
+      <c r="B77" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="C77" s="0" t="s">
+      <c r="C77" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="D77" s="0" t="s">
+      <c r="D77" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="E77" s="0" t="s">
+      <c r="E77" s="1" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+      <c r="A78" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B78" s="0" t="n">
+      <c r="B78" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="C78" s="0" t="s">
+      <c r="C78" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="D78" s="0" t="s">
+      <c r="D78" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="E78" s="0" t="s">
+      <c r="E78" s="1" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+      <c r="A79" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B79" s="0" t="n">
+      <c r="B79" s="1" t="n">
         <v>78</v>
       </c>
-      <c r="C79" s="0" t="s">
+      <c r="C79" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="D79" s="0" t="s">
+      <c r="D79" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="E79" s="0" t="s">
+      <c r="E79" s="1" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
+      <c r="A80" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B80" s="0" t="n">
+      <c r="B80" s="1" t="n">
         <v>79</v>
       </c>
-      <c r="C80" s="0" t="s">
+      <c r="C80" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="D80" s="0" t="s">
+      <c r="D80" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E80" s="0" t="s">
+      <c r="E80" s="1" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
+      <c r="A81" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B81" s="0" t="n">
+      <c r="B81" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="C81" s="0" t="s">
+      <c r="C81" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="D81" s="0" t="s">
+      <c r="D81" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="E81" s="0" t="s">
+      <c r="E81" s="1" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
+      <c r="A82" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B82" s="0" t="n">
+      <c r="B82" s="1" t="n">
         <v>81</v>
       </c>
-      <c r="C82" s="0" t="s">
+      <c r="C82" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="D82" s="0" t="s">
+      <c r="D82" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="E82" s="0" t="s">
+      <c r="E82" s="1" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
+      <c r="A83" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B83" s="0" t="n">
+      <c r="B83" s="1" t="n">
         <v>82</v>
       </c>
-      <c r="C83" s="0" t="s">
+      <c r="C83" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="D83" s="0" t="s">
+      <c r="D83" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E83" s="0" t="s">
+      <c r="E83" s="1" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
+      <c r="A84" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B84" s="0" t="n">
+      <c r="B84" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="C84" s="0" t="s">
+      <c r="C84" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D84" s="0" t="s">
+      <c r="D84" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="E84" s="0" t="s">
+      <c r="E84" s="1" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
+      <c r="A85" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B85" s="0" t="n">
+      <c r="B85" s="1" t="n">
         <v>84</v>
       </c>
-      <c r="C85" s="0" t="s">
+      <c r="C85" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="D85" s="0" t="s">
+      <c r="D85" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="E85" s="0" t="s">
+      <c r="E85" s="1" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
+      <c r="A86" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B86" s="0" t="n">
+      <c r="B86" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="C86" s="0" t="s">
+      <c r="C86" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="D86" s="0" t="s">
+      <c r="D86" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E86" s="0" t="s">
+      <c r="E86" s="1" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
+      <c r="A87" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B87" s="0" t="n">
+      <c r="B87" s="1" t="n">
         <v>86</v>
       </c>
-      <c r="C87" s="0" t="s">
+      <c r="C87" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="D87" s="0" t="s">
+      <c r="D87" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E87" s="0" t="s">
+      <c r="E87" s="1" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
+      <c r="A88" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B88" s="0" t="n">
+      <c r="B88" s="1" t="n">
         <v>87</v>
       </c>
-      <c r="C88" s="0" t="s">
+      <c r="C88" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="D88" s="0" t="s">
+      <c r="D88" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="E88" s="0" t="s">
+      <c r="E88" s="1" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
+      <c r="A89" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B89" s="0" t="n">
+      <c r="B89" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="C89" s="0" t="s">
+      <c r="C89" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="D89" s="0" t="s">
+      <c r="D89" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="E89" s="0" t="s">
+      <c r="E89" s="1" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
+      <c r="A90" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B90" s="0" t="n">
+      <c r="B90" s="1" t="n">
         <v>89</v>
       </c>
-      <c r="C90" s="0" t="s">
+      <c r="C90" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="D90" s="0" t="s">
+      <c r="D90" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="E90" s="0" t="s">
+      <c r="E90" s="1" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="s">
+      <c r="A91" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B91" s="0" t="n">
+      <c r="B91" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="C91" s="0" t="s">
+      <c r="C91" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="D91" s="0" t="s">
+      <c r="D91" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="E91" s="0" t="s">
+      <c r="E91" s="1" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="s">
+      <c r="A92" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B92" s="0" t="n">
+      <c r="B92" s="1" t="n">
         <v>91</v>
       </c>
-      <c r="C92" s="0" t="s">
+      <c r="C92" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="D92" s="0" t="s">
+      <c r="D92" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="E92" s="0" t="s">
+      <c r="E92" s="1" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="s">
+      <c r="A93" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B93" s="0" t="n">
+      <c r="B93" s="1" t="n">
         <v>92</v>
       </c>
-      <c r="C93" s="0" t="s">
+      <c r="C93" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D93" s="0" t="s">
+      <c r="D93" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="E93" s="0" t="s">
+      <c r="E93" s="1" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="s">
+      <c r="A94" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B94" s="0" t="n">
+      <c r="B94" s="1" t="n">
         <v>93</v>
       </c>
-      <c r="C94" s="0" t="s">
+      <c r="C94" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="D94" s="0" t="s">
+      <c r="D94" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="E94" s="0" t="s">
+      <c r="E94" s="1" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="s">
+      <c r="A95" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B95" s="0" t="n">
+      <c r="B95" s="1" t="n">
         <v>94</v>
       </c>
-      <c r="C95" s="0" t="s">
+      <c r="C95" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D95" s="0" t="s">
+      <c r="D95" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="E95" s="0" t="s">
+      <c r="E95" s="1" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="s">
+      <c r="A96" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B96" s="0" t="n">
+      <c r="B96" s="1" t="n">
         <v>95</v>
       </c>
-      <c r="C96" s="0" t="s">
+      <c r="C96" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="D96" s="0" t="s">
+      <c r="D96" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="E96" s="0" t="s">
+      <c r="E96" s="1" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="s">
+      <c r="A97" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B97" s="0" t="n">
+      <c r="B97" s="1" t="n">
         <v>96</v>
       </c>
-      <c r="C97" s="0" t="s">
+      <c r="C97" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="D97" s="0" t="s">
+      <c r="D97" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E97" s="0" t="s">
+      <c r="E97" s="1" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="s">
+      <c r="A98" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B98" s="0" t="n">
+      <c r="B98" s="1" t="n">
         <v>97</v>
       </c>
-      <c r="C98" s="0" t="s">
+      <c r="C98" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="D98" s="0" t="s">
+      <c r="D98" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E98" s="0" t="s">
+      <c r="E98" s="1" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
+      <c r="A99" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B99" s="0" t="n">
+      <c r="B99" s="1" t="n">
         <v>98</v>
       </c>
-      <c r="C99" s="0" t="s">
+      <c r="C99" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="D99" s="0" t="s">
+      <c r="D99" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E99" s="0" t="s">
+      <c r="E99" s="1" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="s">
+      <c r="A100" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B100" s="0" t="n">
+      <c r="B100" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="C100" s="0" t="s">
+      <c r="C100" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="D100" s="0" t="s">
+      <c r="D100" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="E100" s="0" t="s">
+      <c r="E100" s="1" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="s">
+      <c r="A101" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B101" s="0" t="n">
+      <c r="B101" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="C101" s="0" t="s">
+      <c r="C101" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="D101" s="0" t="s">
+      <c r="D101" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="E101" s="0" t="s">
+      <c r="E101" s="1" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="s">
+      <c r="A102" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B102" s="0" t="n">
+      <c r="B102" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="C102" s="0" t="s">
+      <c r="C102" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="D102" s="0" t="s">
+      <c r="D102" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="E102" s="0" t="s">
+      <c r="E102" s="1" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="0" t="s">
+      <c r="A103" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B103" s="0" t="n">
+      <c r="B103" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="C103" s="0" t="s">
+      <c r="C103" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="D103" s="0" t="s">
+      <c r="D103" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="E103" s="0" t="s">
+      <c r="E103" s="1" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
+      <c r="A104" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B104" s="0" t="n">
+      <c r="B104" s="1" t="n">
         <v>103</v>
       </c>
-      <c r="C104" s="0" t="s">
+      <c r="C104" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="D104" s="0" t="s">
+      <c r="D104" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="E104" s="0" t="s">
+      <c r="E104" s="1" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="0" t="s">
+      <c r="A105" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B105" s="0" t="n">
+      <c r="B105" s="1" t="n">
         <v>104</v>
       </c>
-      <c r="C105" s="0" t="s">
+      <c r="C105" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="D105" s="0" t="s">
+      <c r="D105" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E105" s="0" t="s">
+      <c r="E105" s="1" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="0" t="s">
+      <c r="A106" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B106" s="0" t="n">
+      <c r="B106" s="1" t="n">
         <v>105</v>
       </c>
-      <c r="C106" s="0" t="s">
+      <c r="C106" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="D106" s="0" t="s">
+      <c r="D106" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="E106" s="0" t="s">
+      <c r="E106" s="1" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="0" t="s">
+      <c r="A107" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B107" s="0" t="n">
+      <c r="B107" s="1" t="n">
         <v>106</v>
       </c>
-      <c r="C107" s="0" t="s">
+      <c r="C107" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="D107" s="0" t="s">
+      <c r="D107" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="E107" s="0" t="s">
+      <c r="E107" s="1" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="0" t="s">
+      <c r="A108" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B108" s="0" t="n">
+      <c r="B108" s="1" t="n">
         <v>107</v>
       </c>
-      <c r="C108" s="0" t="s">
+      <c r="C108" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="D108" s="0" t="s">
+      <c r="D108" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="E108" s="0" t="s">
+      <c r="E108" s="1" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="s">
+      <c r="A109" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B109" s="0" t="n">
+      <c r="B109" s="1" t="n">
         <v>108</v>
       </c>
-      <c r="C109" s="0" t="s">
+      <c r="C109" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="D109" s="0" t="s">
+      <c r="D109" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="E109" s="0" t="s">
+      <c r="E109" s="1" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="0" t="s">
+      <c r="A110" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B110" s="0" t="n">
+      <c r="B110" s="1" t="n">
         <v>109</v>
       </c>
-      <c r="C110" s="0" t="s">
+      <c r="C110" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="D110" s="0" t="s">
+      <c r="D110" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="E110" s="0" t="s">
+      <c r="E110" s="1" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="0" t="s">
+      <c r="A111" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B111" s="0" t="n">
+      <c r="B111" s="1" t="n">
         <v>110</v>
       </c>
-      <c r="C111" s="0" t="s">
+      <c r="C111" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D111" s="0" t="s">
+      <c r="D111" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="E111" s="0" t="s">
+      <c r="E111" s="1" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="0" t="s">
+      <c r="A112" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B112" s="0" t="n">
+      <c r="B112" s="1" t="n">
         <v>111</v>
       </c>
-      <c r="C112" s="0" t="s">
+      <c r="C112" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D112" s="0" t="s">
+      <c r="D112" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="E112" s="0" t="s">
+      <c r="E112" s="1" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="0" t="s">
+      <c r="A113" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B113" s="0" t="n">
+      <c r="B113" s="1" t="n">
         <v>112</v>
       </c>
-      <c r="C113" s="0" t="s">
+      <c r="C113" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="D113" s="0" t="s">
+      <c r="D113" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="E113" s="0" t="s">
+      <c r="E113" s="1" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="0" t="s">
+      <c r="A114" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B114" s="0" t="n">
+      <c r="B114" s="1" t="n">
         <v>113</v>
       </c>
-      <c r="C114" s="0" t="s">
+      <c r="C114" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="D114" s="0" t="s">
+      <c r="D114" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="E114" s="0" t="s">
+      <c r="E114" s="1" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="0" t="s">
+      <c r="A115" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B115" s="0" t="n">
+      <c r="B115" s="1" t="n">
         <v>114</v>
       </c>
-      <c r="C115" s="0" t="s">
+      <c r="C115" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="D115" s="0" t="s">
+      <c r="D115" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="E115" s="0" t="s">
+      <c r="E115" s="1" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="s">
+      <c r="A116" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B116" s="0" t="n">
+      <c r="B116" s="1" t="n">
         <v>115</v>
       </c>
-      <c r="C116" s="0" t="s">
+      <c r="C116" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="D116" s="0" t="s">
+      <c r="D116" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="E116" s="0" t="s">
+      <c r="E116" s="1" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0" t="s">
+      <c r="A117" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B117" s="0" t="n">
+      <c r="B117" s="1" t="n">
         <v>116</v>
       </c>
-      <c r="C117" s="0" t="s">
+      <c r="C117" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="D117" s="0" t="s">
+      <c r="D117" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="E117" s="0" t="s">
+      <c r="E117" s="1" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="0" t="s">
+      <c r="A118" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B118" s="0" t="n">
+      <c r="B118" s="1" t="n">
         <v>117</v>
       </c>
-      <c r="C118" s="0" t="s">
+      <c r="C118" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="D118" s="0" t="s">
+      <c r="D118" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="E118" s="0" t="s">
+      <c r="E118" s="1" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0" t="s">
+      <c r="A119" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B119" s="0" t="n">
+      <c r="B119" s="1" t="n">
         <v>118</v>
       </c>
-      <c r="C119" s="0" t="s">
+      <c r="C119" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="D119" s="0" t="s">
+      <c r="D119" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="E119" s="0" t="s">
+      <c r="E119" s="1" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="0" t="s">
+      <c r="A120" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B120" s="0" t="n">
+      <c r="B120" s="1" t="n">
         <v>119</v>
       </c>
-      <c r="C120" s="0" t="s">
+      <c r="C120" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="D120" s="0" t="s">
+      <c r="D120" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="E120" s="0" t="s">
+      <c r="E120" s="1" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="0" t="s">
+      <c r="A121" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B121" s="0" t="n">
+      <c r="B121" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="C121" s="0" t="s">
+      <c r="C121" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="D121" s="0" t="s">
+      <c r="D121" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="E121" s="0" t="s">
+      <c r="E121" s="1" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="0" t="s">
+      <c r="A122" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B122" s="0" t="n">
+      <c r="B122" s="1" t="n">
         <v>121</v>
       </c>
-      <c r="C122" s="0" t="s">
+      <c r="C122" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="D122" s="0" t="s">
+      <c r="D122" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="E122" s="0" t="s">
+      <c r="E122" s="1" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="0" t="s">
+      <c r="A123" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B123" s="0" t="n">
+      <c r="B123" s="1" t="n">
         <v>122</v>
       </c>
-      <c r="C123" s="0" t="s">
+      <c r="C123" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="D123" s="0" t="s">
+      <c r="D123" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="E123" s="0" t="s">
+      <c r="E123" s="1" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0" t="s">
+      <c r="A124" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B124" s="0" t="n">
+      <c r="B124" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="C124" s="0" t="s">
+      <c r="C124" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="D124" s="0" t="s">
+      <c r="D124" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="E124" s="0" t="s">
+      <c r="E124" s="1" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="0" t="s">
+      <c r="A125" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B125" s="0" t="n">
+      <c r="B125" s="1" t="n">
         <v>124</v>
       </c>
-      <c r="C125" s="0" t="s">
+      <c r="C125" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="D125" s="0" t="s">
+      <c r="D125" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="E125" s="0" t="s">
+      <c r="E125" s="1" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="0" t="s">
+      <c r="A126" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B126" s="0" t="n">
+      <c r="B126" s="1" t="n">
         <v>125</v>
       </c>
-      <c r="C126" s="0" t="s">
+      <c r="C126" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="D126" s="0" t="s">
+      <c r="D126" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="E126" s="0" t="s">
+      <c r="E126" s="1" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="0" t="s">
+      <c r="A127" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B127" s="0" t="n">
+      <c r="B127" s="1" t="n">
         <v>126</v>
       </c>
-      <c r="C127" s="0" t="s">
+      <c r="C127" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="D127" s="0" t="s">
+      <c r="D127" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="E127" s="0" t="s">
+      <c r="E127" s="1" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="0" t="s">
+      <c r="A128" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B128" s="0" t="n">
+      <c r="B128" s="1" t="n">
         <v>127</v>
       </c>
-      <c r="C128" s="0" t="s">
+      <c r="C128" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="D128" s="0" t="s">
+      <c r="D128" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="E128" s="0" t="s">
+      <c r="E128" s="1" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="0" t="s">
+      <c r="A129" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B129" s="0" t="n">
+      <c r="B129" s="1" t="n">
         <v>128</v>
       </c>
-      <c r="C129" s="0" t="s">
+      <c r="C129" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="D129" s="0" t="s">
+      <c r="D129" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="E129" s="0" t="s">
+      <c r="E129" s="1" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="0" t="s">
+      <c r="A130" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B130" s="0" t="n">
+      <c r="B130" s="1" t="n">
         <v>129</v>
       </c>
-      <c r="C130" s="0" t="s">
+      <c r="C130" s="1" t="s">
         <v>324</v>
       </c>
-      <c r="D130" s="0" t="s">
+      <c r="D130" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="E130" s="0" t="s">
+      <c r="E130" s="1" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="0" t="s">
+      <c r="A131" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B131" s="0" t="n">
+      <c r="B131" s="1" t="n">
         <v>130</v>
       </c>
-      <c r="C131" s="0" t="s">
+      <c r="C131" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="D131" s="0" t="s">
+      <c r="D131" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="E131" s="0" t="s">
+      <c r="E131" s="1" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="0" t="s">
+      <c r="A132" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B132" s="0" t="n">
+      <c r="B132" s="1" t="n">
         <v>131</v>
       </c>
-      <c r="C132" s="0" t="s">
+      <c r="C132" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="D132" s="0" t="s">
+      <c r="D132" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="E132" s="0" t="s">
+      <c r="E132" s="1" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="0" t="s">
+      <c r="A133" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B133" s="0" t="n">
+      <c r="B133" s="1" t="n">
         <v>132</v>
       </c>
-      <c r="C133" s="0" t="s">
+      <c r="C133" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="D133" s="0" t="s">
+      <c r="D133" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="E133" s="0" t="s">
+      <c r="E133" s="1" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="0" t="s">
+      <c r="A134" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B134" s="0" t="n">
+      <c r="B134" s="1" t="n">
         <v>133</v>
       </c>
-      <c r="C134" s="0" t="s">
+      <c r="C134" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="D134" s="0" t="s">
+      <c r="D134" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="E134" s="0" t="s">
+      <c r="E134" s="1" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="0" t="s">
+      <c r="A135" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B135" s="0" t="n">
+      <c r="B135" s="1" t="n">
         <v>134</v>
       </c>
-      <c r="C135" s="0" t="s">
+      <c r="C135" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="D135" s="0" t="s">
+      <c r="D135" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="E135" s="0" t="s">
+      <c r="E135" s="1" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="0" t="s">
+      <c r="A136" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B136" s="0" t="n">
+      <c r="B136" s="1" t="n">
         <v>135</v>
       </c>
-      <c r="C136" s="0" t="s">
+      <c r="C136" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="D136" s="0" t="s">
+      <c r="D136" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="E136" s="0" t="s">
+      <c r="E136" s="1" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="0" t="s">
+      <c r="A137" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B137" s="0" t="n">
+      <c r="B137" s="1" t="n">
         <v>136</v>
       </c>
-      <c r="C137" s="0" t="s">
+      <c r="C137" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="D137" s="0" t="s">
+      <c r="D137" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="E137" s="0" t="s">
+      <c r="E137" s="1" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="0" t="s">
+      <c r="A138" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B138" s="0" t="n">
+      <c r="B138" s="1" t="n">
         <v>137</v>
       </c>
-      <c r="C138" s="0" t="s">
+      <c r="C138" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="D138" s="0" t="s">
+      <c r="D138" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="E138" s="0" t="s">
+      <c r="E138" s="1" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="0" t="s">
+      <c r="A139" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B139" s="0" t="n">
+      <c r="B139" s="1" t="n">
         <v>138</v>
       </c>
-      <c r="C139" s="0" t="s">
+      <c r="C139" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="D139" s="0" t="s">
+      <c r="D139" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="E139" s="0" t="s">
+      <c r="E139" s="1" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="0" t="s">
+      <c r="A140" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B140" s="0" t="n">
+      <c r="B140" s="1" t="n">
         <v>139</v>
       </c>
-      <c r="C140" s="0" t="s">
+      <c r="C140" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="D140" s="0" t="s">
+      <c r="D140" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="E140" s="0" t="s">
+      <c r="E140" s="1" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="0" t="s">
+      <c r="A141" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B141" s="0" t="n">
+      <c r="B141" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="C141" s="0" t="s">
+      <c r="C141" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="D141" s="0" t="s">
+      <c r="D141" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="E141" s="0" t="s">
+      <c r="E141" s="1" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="0" t="s">
+      <c r="A142" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B142" s="0" t="n">
+      <c r="B142" s="1" t="n">
         <v>141</v>
       </c>
-      <c r="C142" s="0" t="s">
+      <c r="C142" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="D142" s="0" t="s">
+      <c r="D142" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="E142" s="0" t="s">
+      <c r="E142" s="1" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="0" t="s">
+      <c r="A143" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B143" s="0" t="n">
+      <c r="B143" s="1" t="n">
         <v>142</v>
       </c>
-      <c r="C143" s="0" t="s">
+      <c r="C143" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="D143" s="0" t="s">
+      <c r="D143" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="E143" s="0" t="s">
+      <c r="E143" s="1" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="0" t="s">
+      <c r="A144" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B144" s="0" t="n">
+      <c r="B144" s="1" t="n">
         <v>143</v>
       </c>
-      <c r="C144" s="0" t="s">
+      <c r="C144" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="D144" s="0" t="s">
+      <c r="D144" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="E144" s="0" t="s">
+      <c r="E144" s="1" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="0" t="s">
+      <c r="A145" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B145" s="0" t="n">
+      <c r="B145" s="1" t="n">
         <v>144</v>
       </c>
-      <c r="C145" s="0" t="s">
+      <c r="C145" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="D145" s="0" t="s">
+      <c r="D145" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="E145" s="0" t="s">
+      <c r="E145" s="1" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="0" t="s">
+      <c r="A146" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B146" s="0" t="n">
+      <c r="B146" s="1" t="n">
         <v>145</v>
       </c>
-      <c r="C146" s="0" t="s">
+      <c r="C146" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="D146" s="0" t="s">
+      <c r="D146" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="E146" s="0" t="s">
+      <c r="E146" s="1" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="0" t="s">
+      <c r="A147" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B147" s="0" t="n">
+      <c r="B147" s="1" t="n">
         <v>146</v>
       </c>
-      <c r="C147" s="0" t="s">
+      <c r="C147" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="D147" s="0" t="s">
+      <c r="D147" s="1" t="s">
         <v>369</v>
       </c>
-      <c r="E147" s="0" t="s">
+      <c r="E147" s="1" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="0" t="s">
+      <c r="A148" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B148" s="0" t="n">
+      <c r="B148" s="1" t="n">
         <v>147</v>
       </c>
-      <c r="C148" s="0" t="s">
+      <c r="C148" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="D148" s="0" t="s">
+      <c r="D148" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="E148" s="0" t="s">
+      <c r="E148" s="1" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="0" t="s">
+      <c r="A149" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="B149" s="0" t="n">
+      <c r="B149" s="1" t="n">
         <v>148</v>
       </c>
-      <c r="C149" s="0" t="s">
+      <c r="C149" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="D149" s="0" t="s">
+      <c r="D149" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="E149" s="0" t="s">
+      <c r="E149" s="1" t="s">
         <v>372</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed formatting for mobile phones and modified some display issues.
</commit_message>
<xml_diff>
--- a/Situations-n-Resolutions-with-sections.xlsx
+++ b/Situations-n-Resolutions-with-sections.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Applicable Rule</t>
   </si>
   <si>
-    <t xml:space="preserve">Officiating Athletes with Disabilities</t>
+    <t xml:space="preserve">ᐧ Disabilities</t>
   </si>
   <si>
     <t xml:space="preserve">A swimmer with a disability is entered in a meet. When sending in the team’s entries, their coach informed the entry chair of the swimmer’s disability using a Necessary Accommodation form. What happens now?</t>
@@ -1381,18 +1381,18 @@
   <dimension ref="A1:E149"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C71" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A71" activeCellId="0" sqref="A71"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="64.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="64.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="67.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="122.05"/>

</xml_diff>